<commit_message>
Apply weaponDB to weapon
</commit_message>
<xml_diff>
--- a/Assets/7. DataBase/DataBase.xlsx
+++ b/Assets/7. DataBase/DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\Codename\Assets\7. DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4944AC-13A0-4E38-803D-82AA502DA8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030FEC1F-8225-4362-BE8F-C53507023720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-2730" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{4EE84E4A-F28B-4CEA-A4E3-45FAF769CEDC}"/>
+    <workbookView xWindow="38280" yWindow="-2895" windowWidth="16440" windowHeight="28320" xr2:uid="{4EE84E4A-F28B-4CEA-A4E3-45FAF769CEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="WeaponDB" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>weaponID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,6 +65,70 @@
   </si>
   <si>
     <t>enemyID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RifleA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RifleS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RifleB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RifleC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PistolS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PistolA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PistolB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PistolC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SnipeS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SnipeA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SnipeB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SnipeC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShotgunS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShotgunA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShotgunB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShotgunC1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,13 +493,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCD5F2D-2FAF-44DF-ACAF-69D2B98DE5FA}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -458,17 +525,17 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>0.1</v>
@@ -478,17 +545,17 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>0.2</v>
@@ -498,17 +565,17 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>0.3</v>
@@ -518,8 +585,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>13</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -534,6 +601,246 @@
         <v>0.4</v>
       </c>
       <c r="F5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>1.5</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1.5</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1.5</v>
+      </c>
+      <c r="F12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>1.5</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>40</v>
       </c>
     </row>
@@ -547,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFFE5D8-5A58-468A-BA77-83AAB1C95324}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Apply Enemy DB to Enemy
</commit_message>
<xml_diff>
--- a/Assets/7. DataBase/DataBase.xlsx
+++ b/Assets/7. DataBase/DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\Codename\Assets\7. DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030FEC1F-8225-4362-BE8F-C53507023720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D1EDFF-92FB-4AAF-9C07-D93B7093E630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-2895" windowWidth="16440" windowHeight="28320" xr2:uid="{4EE84E4A-F28B-4CEA-A4E3-45FAF769CEDC}"/>
+    <workbookView xWindow="38280" yWindow="-2895" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{4EE84E4A-F28B-4CEA-A4E3-45FAF769CEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="WeaponDB" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>weaponID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,19 +52,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>itemProp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>speed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>health</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemyID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -495,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCD5F2D-2FAF-44DF-ACAF-69D2B98DE5FA}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -526,7 +518,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -546,7 +538,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -566,7 +558,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -586,7 +578,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -606,7 +598,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>30</v>
@@ -626,7 +618,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -646,7 +638,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -666,7 +658,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -686,7 +678,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -706,7 +698,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -726,7 +718,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -746,7 +738,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -766,7 +758,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -786,7 +778,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -806,7 +798,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -826,7 +818,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -854,24 +846,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFFE5D8-5A58-468A-BA77-83AAB1C95324}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Balancing Fetch Boss & Weapon & Enemy
</commit_message>
<xml_diff>
--- a/Assets/7. DataBase/DataBase.xlsx
+++ b/Assets/7. DataBase/DataBase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\Codename\Assets\7. DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D1EDFF-92FB-4AAF-9C07-D93B7093E630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F3273F-227E-4FF5-AEDB-153E17F2B3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-2895" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{4EE84E4A-F28B-4CEA-A4E3-45FAF769CEDC}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -521,19 +521,19 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -541,19 +541,19 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -561,19 +561,19 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -581,19 +581,19 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="F5">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -601,19 +601,19 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -621,19 +621,19 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F7">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -644,16 +644,16 @@
         <v>20</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -664,16 +664,16 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -681,19 +681,19 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C10">
+        <v>1.5</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>1.5</v>
-      </c>
       <c r="F10">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -701,19 +701,19 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -721,19 +721,19 @@
         <v>18</v>
       </c>
       <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>2.5</v>
+      </c>
+      <c r="D12">
         <v>6</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
       </c>
       <c r="E12">
         <v>1.5</v>
       </c>
       <c r="F12">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -741,19 +741,19 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="F13">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -761,19 +761,19 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -781,19 +781,19 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F15">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -801,19 +801,19 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F16">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -821,19 +821,19 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -847,7 +847,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -868,13 +868,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -882,27 +882,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -910,13 +910,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>4</v>

</xml_diff>